<commit_message>
add predictions + logboek joey
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek Joey.xlsx
+++ b/Documents/Logboeken/Logboek Joey.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -109,9 +109,6 @@
     <t>Week 2</t>
   </si>
   <si>
-    <t>Maandag</t>
-  </si>
-  <si>
     <t>wireframes aangepast</t>
   </si>
   <si>
@@ -122,6 +119,30 @@
   </si>
   <si>
     <t>morgen kijken noël en Ik verder naar een oplossing</t>
+  </si>
+  <si>
+    <t>woensdag</t>
+  </si>
+  <si>
+    <t>maandag</t>
+  </si>
+  <si>
+    <t>dinsdag</t>
+  </si>
+  <si>
+    <t>Dondaerdag</t>
+  </si>
+  <si>
+    <t>gekeken met noël naar wireframes</t>
+  </si>
+  <si>
+    <t>aan c# voor applicate gewerkt</t>
+  </si>
+  <si>
+    <t>kaan gevraagd wat hij deed</t>
+  </si>
+  <si>
+    <t>we hebben hem een html taak gegeven</t>
   </si>
 </sst>
 </file>
@@ -495,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +648,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3">
         <v>0.57986111111111105</v>
@@ -636,35 +657,88 @@
         <v>330</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E19">
+        <v>330</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3">
         <v>0.5625</v>
       </c>
-      <c r="E19">
-        <v>330</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="E21">
+        <v>330</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E22">
+        <v>330</v>
+      </c>
+      <c r="G22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C20" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="E20">
-        <v>330</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="N22" t="s">
         <v>27</v>
       </c>
-      <c r="N20" t="s">
-        <v>28</v>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E24">
+        <v>330</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E25">
+        <v>330</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C26" s="3">
+        <v>0.45902777777777781</v>
+      </c>
+      <c r="E26">
+        <v>330</v>
+      </c>
+      <c r="G26" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add c# + Logboek Joey
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek Joey.xlsx
+++ b/Documents/Logboeken/Logboek Joey.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -522,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,6 +835,23 @@
         <v>31</v>
       </c>
     </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E33">
+        <v>330</v>
+      </c>
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>